<commit_message>
design add jr and jal
</commit_message>
<xml_diff>
--- a/doc/truth-table.xlsx
+++ b/doc/truth-table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PipelineCPU\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A07DEE-55C0-498E-B3DA-C5425B7D69A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F606F6A-CEE3-4397-9B2C-3F2F33FF289C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="1215" windowWidth="13980" windowHeight="14985" xr2:uid="{916343F6-8B66-43CC-B58B-80C742A562DC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="136">
   <si>
     <t>add</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -524,6 +524,46 @@
   </si>
   <si>
     <t>inst</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jal_br</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>off</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>on</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jr_br</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -578,7 +618,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -590,6 +630,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -905,9 +948,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06DDC9C-5083-4640-915A-C7C0E11715ED}">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
@@ -2321,84 +2366,87 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A39" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>110</v>
+      <c r="A39" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>80</v>
+        <v>128</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A40" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>112</v>
+      <c r="A40" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>81</v>
+        <v>135</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
-        <v>119</v>
+        <v>35</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>48</v>
@@ -2427,36 +2475,106 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A43" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L42" s="1" t="s">
+      <c r="E44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L44" s="1" t="s">
         <v>121</v>
       </c>
     </row>

</xml_diff>